<commit_message>
Updated perovskite_ions excel sheet to use X instead of C
</commit_message>
<xml_diff>
--- a/tests/data/perovskite_ions.xlsx
+++ b/tests/data/perovskite_ions.xlsx
@@ -8053,7 +8053,7 @@
     <t xml:space="preserve">16065-91-1</t>
   </si>
   <si>
-    <t xml:space="preserve">C</t>
+    <t xml:space="preserve">X</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
@@ -9067,8 +9067,8 @@
   </sheetPr>
   <dimension ref="A1:N336"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A304" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B328" activeCellId="0" sqref="B328:B336"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A259" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B336" activeCellId="0" sqref="B336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Corrected molecular formula for TT and DTT in excel sheet
</commit_message>
<xml_diff>
--- a/tests/data/perovskite_ions.xlsx
+++ b/tests/data/perovskite_ions.xlsx
@@ -5877,7 +5877,7 @@
     <t xml:space="preserve">TT</t>
   </si>
   <si>
-    <t xml:space="preserve">C22H20NS5+</t>
+    <t xml:space="preserve">C22H22NS5+</t>
   </si>
   <si>
     <t xml:space="preserve">[NH3+]CCc1ccc(s1)C1C=C(C)C(S1)c1sc2cc(sc2c1)c1sccc1C</t>
@@ -5898,7 +5898,7 @@
     <t xml:space="preserve">DTT</t>
   </si>
   <si>
-    <t xml:space="preserve">C24H20NS6+</t>
+    <t xml:space="preserve">C24H22NS6+</t>
   </si>
   <si>
     <t xml:space="preserve">[NH3+]CCc1ccc(s1)C1C=C(C)C(S1)c1sc2c3sc(cc3sc2c1)c1sccc1C</t>
@@ -9067,8 +9067,8 @@
   </sheetPr>
   <dimension ref="A1:N336"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A259" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B336" activeCellId="0" sqref="B336"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E230" activeCellId="0" sqref="E230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Corrected molecular formula for TT and DTT in excel sheet (#45)
</commit_message>
<xml_diff>
--- a/tests/data/perovskite_ions.xlsx
+++ b/tests/data/perovskite_ions.xlsx
@@ -5877,7 +5877,7 @@
     <t xml:space="preserve">TT</t>
   </si>
   <si>
-    <t xml:space="preserve">C22H20NS5+</t>
+    <t xml:space="preserve">C22H22NS5+</t>
   </si>
   <si>
     <t xml:space="preserve">[NH3+]CCc1ccc(s1)C1C=C(C)C(S1)c1sc2cc(sc2c1)c1sccc1C</t>
@@ -5898,7 +5898,7 @@
     <t xml:space="preserve">DTT</t>
   </si>
   <si>
-    <t xml:space="preserve">C24H20NS6+</t>
+    <t xml:space="preserve">C24H22NS6+</t>
   </si>
   <si>
     <t xml:space="preserve">[NH3+]CCc1ccc(s1)C1C=C(C)C(S1)c1sc2c3sc(cc3sc2c1)c1sccc1C</t>
@@ -9067,8 +9067,8 @@
   </sheetPr>
   <dimension ref="A1:N336"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A259" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B336" activeCellId="0" sqref="B336"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E230" activeCellId="0" sqref="E230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>